<commit_message>
fix loi chuc nang sua thong tin giang vien: doi role
</commit_message>
<xml_diff>
--- a/uet-portal-backend/uploads/danh_sach_hoc_vien_them_khoa.xlsx
+++ b/uet-portal-backend/uploads/danh_sach_hoc_vien_them_khoa.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UET\KLTN3\KLTN\uet-portal-backend\uploads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3913BC0-A66E-4F2B-A77D-D8E227EDB808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -685,8 +691,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,13 +755,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -793,7 +807,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -827,6 +841,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -861,9 +876,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1036,14 +1052,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>21020192</v>
       </c>
@@ -1077,7 +1102,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>31937560</v>
       </c>
@@ -1094,7 +1119,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>52165286</v>
       </c>
@@ -1111,7 +1136,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>59368624</v>
       </c>
@@ -1128,7 +1153,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>72409550</v>
       </c>
@@ -1145,7 +1170,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>42947565</v>
       </c>
@@ -1162,7 +1187,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>60296437</v>
       </c>
@@ -1179,7 +1204,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>14776315</v>
       </c>
@@ -1196,7 +1221,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>32575861</v>
       </c>
@@ -1213,7 +1238,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>80607767</v>
       </c>
@@ -1230,7 +1255,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>16893769</v>
       </c>
@@ -1247,7 +1272,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>81044514</v>
       </c>
@@ -1264,7 +1289,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>22919390</v>
       </c>
@@ -1281,7 +1306,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11521881</v>
       </c>
@@ -1298,7 +1323,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>45972556</v>
       </c>
@@ -1315,7 +1340,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>32254964</v>
       </c>
@@ -1332,7 +1357,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>32036693</v>
       </c>
@@ -1349,7 +1374,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>67567585</v>
       </c>
@@ -1366,7 +1391,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>26695019</v>
       </c>
@@ -1383,7 +1408,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>56691452</v>
       </c>
@@ -1400,7 +1425,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>52254490</v>
       </c>
@@ -1417,7 +1442,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>80985291</v>
       </c>
@@ -1434,7 +1459,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>84405178</v>
       </c>
@@ -1451,7 +1476,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>56435953</v>
       </c>
@@ -1468,7 +1493,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>62557456</v>
       </c>
@@ -1485,7 +1510,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>48142448</v>
       </c>
@@ -1502,7 +1527,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>31426241</v>
       </c>
@@ -1519,7 +1544,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>68370934</v>
       </c>
@@ -1536,7 +1561,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>51395162</v>
       </c>
@@ -1553,7 +1578,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>86094463</v>
       </c>
@@ -1570,7 +1595,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>96530989</v>
       </c>
@@ -1587,7 +1612,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>67879455</v>
       </c>
@@ -1604,7 +1629,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>86490884</v>
       </c>
@@ -1621,7 +1646,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>57256804</v>
       </c>
@@ -1638,7 +1663,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>40592464</v>
       </c>
@@ -1655,7 +1680,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>16217346</v>
       </c>
@@ -1672,7 +1697,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20781298</v>
       </c>
@@ -1689,7 +1714,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>63733965</v>
       </c>
@@ -1706,7 +1731,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>59315285</v>
       </c>
@@ -1723,7 +1748,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>22182764</v>
       </c>
@@ -1740,7 +1765,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>53366176</v>
       </c>
@@ -1757,7 +1782,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>30971664</v>
       </c>
@@ -1774,7 +1799,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>14688586</v>
       </c>
@@ -1791,7 +1816,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>99090313</v>
       </c>
@@ -1808,7 +1833,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>24390564</v>
       </c>
@@ -1825,7 +1850,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>51048635</v>
       </c>
@@ -1842,7 +1867,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>92097141</v>
       </c>
@@ -1859,7 +1884,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>30258427</v>
       </c>
@@ -1876,7 +1901,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>92650137</v>
       </c>
@@ -1893,7 +1918,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>89230970</v>
       </c>
@@ -1910,7 +1935,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>82411299</v>
       </c>
@@ -1927,7 +1952,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>19144028</v>
       </c>
@@ -1944,7 +1969,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>94133139</v>
       </c>
@@ -1961,7 +1986,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>21301430</v>
       </c>
@@ -1978,7 +2003,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>77418474</v>
       </c>
@@ -1995,7 +2020,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>96934503</v>
       </c>
@@ -2012,7 +2037,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>39942058</v>
       </c>
@@ -2029,7 +2054,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>87348953</v>
       </c>
@@ -2046,7 +2071,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>49572803</v>
       </c>
@@ -2063,7 +2088,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60062201</v>
       </c>
@@ -2080,7 +2105,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>83860908</v>
       </c>
@@ -2097,7 +2122,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>42573155</v>
       </c>
@@ -2114,7 +2139,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>82082240</v>
       </c>
@@ -2131,7 +2156,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>81832018</v>
       </c>
@@ -2148,7 +2173,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>11398556</v>
       </c>
@@ -2165,7 +2190,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>89190179</v>
       </c>
@@ -2182,7 +2207,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>55256024</v>
       </c>
@@ -2199,7 +2224,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>66798320</v>
       </c>
@@ -2216,7 +2241,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>30196080</v>
       </c>
@@ -2233,7 +2258,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>13179105</v>
       </c>
@@ -2250,7 +2275,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>32498317</v>
       </c>
@@ -2267,7 +2292,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>70153516</v>
       </c>
@@ -2284,7 +2309,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>62021007</v>
       </c>
@@ -2301,7 +2326,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>16021478</v>
       </c>
@@ -2318,7 +2343,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>60442899</v>
       </c>
@@ -2335,7 +2360,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>48523840</v>
       </c>
@@ -2352,7 +2377,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>52470379</v>
       </c>
@@ -2369,7 +2394,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>33636496</v>
       </c>
@@ -2386,7 +2411,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>69306592</v>
       </c>
@@ -2403,7 +2428,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>70534958</v>
       </c>
@@ -2420,7 +2445,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>65287094</v>
       </c>
@@ -2437,7 +2462,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>37649529</v>
       </c>
@@ -2454,7 +2479,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>43570795</v>
       </c>
@@ -2471,7 +2496,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>58285090</v>
       </c>
@@ -2488,7 +2513,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>11125750</v>
       </c>
@@ -2505,7 +2530,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>39697280</v>
       </c>
@@ -2522,7 +2547,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>89806187</v>
       </c>
@@ -2539,7 +2564,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>47102579</v>
       </c>
@@ -2556,7 +2581,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>66923958</v>
       </c>
@@ -2573,7 +2598,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>28379567</v>
       </c>
@@ -2590,7 +2615,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>72635906</v>
       </c>
@@ -2607,7 +2632,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>97770454</v>
       </c>
@@ -2624,7 +2649,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>53773953</v>
       </c>
@@ -2641,7 +2666,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>70056992</v>
       </c>
@@ -2658,7 +2683,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>69060854</v>
       </c>
@@ -2675,7 +2700,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>66781896</v>
       </c>
@@ -2692,7 +2717,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>48259317</v>
       </c>
@@ -2709,7 +2734,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>46033577</v>
       </c>
@@ -2726,7 +2751,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>36387775</v>
       </c>
@@ -2743,7 +2768,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>38979823</v>
       </c>
@@ -2760,7 +2785,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>92488791</v>
       </c>

</xml_diff>